<commit_message>
Massive changes to the  Create Material Symbols tool
</commit_message>
<xml_diff>
--- a/BARevitTools/Resources/SYMB Material List.xlsx
+++ b/BARevitTools/Resources/SYMB Material List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clicea\OneDrive\Documents\CSharp\UITests\UITests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clicea\OneDrive\Documents\CSharp\BARevitTools\BARevitTools\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B8E0BC2B-9C55-49F6-B1ED-3456FE60315B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B9257F54-66A2-421C-A9C3-C182AA600068}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{B8E0BC2B-9C55-49F6-B1ED-3456FE60315B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{AD01F943-C0F3-4526-87A8-E23CA1831980}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mat List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID Use</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Color / Style</t>
+  </si>
+  <si>
+    <t>Include In Material List</t>
   </si>
 </sst>
 </file>
@@ -601,15 +604,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F1EA4A5-D6B7-4AE6-BFE7-A8F7D043E9F0}" name="Table1" displayName="Table1" ref="A1:J3" totalsRowShown="0">
-  <autoFilter ref="A1:J3" xr:uid="{6DDD47BD-B7BA-4094-9C18-D08E71C29A97}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F1EA4A5-D6B7-4AE6-BFE7-A8F7D043E9F0}" name="Table1" displayName="Table1" ref="A1:K3" totalsRowShown="0">
+  <autoFilter ref="A1:K3" xr:uid="{6DDD47BD-B7BA-4094-9C18-D08E71C29A97}">
     <filterColumn colId="1">
       <filters>
         <filter val="CASEWORK"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{40E5ECBA-4CEE-4C1A-BDEF-9EBE29B9D390}" name="Type"/>
     <tableColumn id="2" xr3:uid="{52C50076-B1B5-4FEB-ADFE-8D5E527483E9}" name="ID Use"/>
     <tableColumn id="3" xr3:uid="{65ACE578-7EF2-4446-A437-23797B7E44E3}" name="Mark"/>
@@ -620,6 +623,7 @@
     <tableColumn id="8" xr3:uid="{BDA6BAA9-14DC-4760-B97D-5ECC576AD573}" name="VOC Compliance"/>
     <tableColumn id="9" xr3:uid="{B1507BDF-0407-4D32-8FF9-68D2F5C4FCEC}" name="Fire Rating"/>
     <tableColumn id="10" xr3:uid="{D72F1FA1-2532-47A5-A485-2F551D131B77}" name="Contact Info"/>
+    <tableColumn id="11" xr3:uid="{D47DD16C-467F-4B94-BE4E-EA9A848A98D8}" name="Include In Material List"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -888,26 +892,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.36328125" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.08984375" customWidth="1"/>
-    <col min="7" max="7" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -937,6 +942,9 @@
       </c>
       <c r="J1" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>